<commit_message>
Add Zip Code Distance Calculator using Streamlit and Haversine formula
</commit_message>
<xml_diff>
--- a/data/New Install Billing Worksheet January.xlsx
+++ b/data/New Install Billing Worksheet January.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Library/CloudStorage/Dropbox/Business/Brendamour_Logistics/BMAY_Pricing_Calc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DAACCCA-9AAF-0540-913C-21D4A2F5E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D36494-B344-A945-9D09-4BFE8B23A287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="33360" windowHeight="36120" xr2:uid="{842D8625-044E-4A8B-B232-483F459CF4B2}"/>
   </bookViews>
@@ -8536,7 +8536,7 @@
     <t>Cat5 cable</t>
   </si>
   <si>
-    <t>Miles From 45241</t>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -9016,7 +9016,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="78" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>